<commit_message>
Validation now working for updateCategories.php
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E952899D-5728-4708-B02F-4C910F70178A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88314457-D07A-4C7B-8A32-27D9C1B4B58F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2015" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
   <si>
     <t/>
   </si>
@@ -33,12 +33,6 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Income Tax Expense</t>
-  </si>
-  <si>
-    <t>Administrative Expenses</t>
-  </si>
-  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
@@ -78,27 +72,15 @@
     <t>Accounting fee</t>
   </si>
   <si>
-    <t>Cost of Sales</t>
-  </si>
-  <si>
     <t>Purchases</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>Retained Profits</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
-    <t>Share Capital</t>
-  </si>
-  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
@@ -108,9 +90,6 @@
     <t>Accruals</t>
   </si>
   <si>
-    <t>GST Payables</t>
-  </si>
-  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -120,9 +99,6 @@
     <t>GST Collected</t>
   </si>
   <si>
-    <t>Trade Payables</t>
-  </si>
-  <si>
     <t>Trade Payables - USD Exchange</t>
   </si>
   <si>
@@ -132,15 +108,9 @@
     <t>Prepayments</t>
   </si>
   <si>
-    <t>Deposits</t>
-  </si>
-  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
-    <t>Plant and Equipment</t>
-  </si>
-  <si>
     <t>Softwares Accum Dep'n</t>
   </si>
   <si>
@@ -153,18 +123,12 @@
     <t>Office Equipment at Cost</t>
   </si>
   <si>
-    <t>Trade Receivables</t>
-  </si>
-  <si>
     <t>Trade Receivables - USD Exchan</t>
   </si>
   <si>
     <t>Trade Receivables - USD</t>
   </si>
   <si>
-    <t>Bank Balances</t>
-  </si>
-  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -183,15 +147,6 @@
     <t>Account</t>
   </si>
   <si>
-    <t>Trial Balance</t>
-  </si>
-  <si>
-    <t>VSIG Pte. Ltd.</t>
-  </si>
-  <si>
-    <t>December 2015</t>
-  </si>
-  <si>
     <t>Amount owing to directors</t>
   </si>
   <si>
@@ -210,58 +165,10 @@
     <t>Skill Development Levy</t>
   </si>
   <si>
-    <t>Amount owing to a Shareholder</t>
-  </si>
-  <si>
-    <t>Income Tax Payables</t>
-  </si>
-  <si>
     <t>Administrative expenses</t>
   </si>
   <si>
     <t>Freight paid</t>
-  </si>
-  <si>
-    <t>Exchange Gain - Trade</t>
-  </si>
-  <si>
-    <t>Exchange Gain - Non-trade</t>
-  </si>
-  <si>
-    <t>Accounting Fee</t>
-  </si>
-  <si>
-    <t>Compilation Fee</t>
-  </si>
-  <si>
-    <t>Freight Charges</t>
-  </si>
-  <si>
-    <t>Internet Expenses</t>
-  </si>
-  <si>
-    <t>Late Penalty</t>
-  </si>
-  <si>
-    <t>Nominee Director Fee</t>
-  </si>
-  <si>
-    <t>Postage and Courier</t>
-  </si>
-  <si>
-    <t>Salaries</t>
-  </si>
-  <si>
-    <t>Secretarial Fee</t>
-  </si>
-  <si>
-    <t>Skill Development Levy &amp; SINDA</t>
-  </si>
-  <si>
-    <t>Taxation Fee</t>
-  </si>
-  <si>
-    <t>Telephone Expenses</t>
   </si>
   <si>
     <t>Income tax expenses</t>
@@ -272,9 +179,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -481,84 +388,84 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,22 +474,22 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -591,49 +498,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -958,7 +865,7 @@
   <dimension ref="A1:AA68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1387,9 +1294,7 @@
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="16" t="s">
-        <v>53</v>
-      </c>
+      <c r="E2" s="16"/>
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
       <c r="H2" s="60"/>
@@ -1418,9 +1323,7 @@
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="22"/>
       <c r="F3" s="23"/>
       <c r="G3" s="24"/>
       <c r="H3" s="60"/>
@@ -1449,9 +1352,7 @@
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="D4" s="21"/>
-      <c r="E4" s="22" t="s">
-        <v>0</v>
-      </c>
+      <c r="E4" s="22"/>
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
       <c r="H4" s="60"/>
@@ -1480,9 +1381,7 @@
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="22" t="s">
-        <v>0</v>
-      </c>
+      <c r="E5" s="22"/>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
       <c r="H5" s="60"/>
@@ -1511,9 +1410,7 @@
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="22" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="22"/>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
       <c r="H6" s="60"/>
@@ -1542,9 +1439,7 @@
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="E7" s="26"/>
       <c r="F7" s="27"/>
       <c r="G7" s="28"/>
       <c r="H7" s="60"/>
@@ -1573,9 +1468,7 @@
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="29" t="s">
-        <v>54</v>
-      </c>
+      <c r="E8" s="29"/>
       <c r="F8" s="27"/>
       <c r="G8" s="30"/>
       <c r="H8" s="60"/>
@@ -1634,15 +1527,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="38" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="41"/>
@@ -1671,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="45"/>
@@ -1679,9 +1572,7 @@
         <v>442930.78</v>
       </c>
       <c r="G11" s="46"/>
-      <c r="H11" s="58" t="s">
-        <v>45</v>
-      </c>
+      <c r="H11" s="58"/>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="47"/>
@@ -1708,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D12" s="45"/>
       <c r="E12" s="45"/>
@@ -1716,9 +1607,7 @@
         <v>399973.51</v>
       </c>
       <c r="G12" s="46"/>
-      <c r="H12" s="58" t="s">
-        <v>45</v>
-      </c>
+      <c r="H12" s="58"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -1745,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -1753,9 +1642,7 @@
         <v>165789.01999999999</v>
       </c>
       <c r="G13" s="46"/>
-      <c r="H13" s="58" t="s">
-        <v>45</v>
-      </c>
+      <c r="H13" s="58"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -1782,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
@@ -1790,9 +1677,7 @@
         <v>325522.73</v>
       </c>
       <c r="G14" s="46"/>
-      <c r="H14" s="58" t="s">
-        <v>42</v>
-      </c>
+      <c r="H14" s="58"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1819,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
@@ -1827,9 +1712,7 @@
         <v>134929.18</v>
       </c>
       <c r="G15" s="46"/>
-      <c r="H15" s="58" t="s">
-        <v>42</v>
-      </c>
+      <c r="H15" s="58"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -1856,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
@@ -1864,9 +1747,7 @@
         <v>1368</v>
       </c>
       <c r="G16" s="46"/>
-      <c r="H16" s="58" t="s">
-        <v>37</v>
-      </c>
+      <c r="H16" s="58"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -1892,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
@@ -1900,16 +1781,14 @@
       <c r="G17" s="62">
         <v>456</v>
       </c>
-      <c r="H17" s="58" t="s">
-        <v>37</v>
-      </c>
+      <c r="H17" s="58"/>
     </row>
     <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
@@ -1917,16 +1796,14 @@
         <v>7607.43</v>
       </c>
       <c r="G18" s="46"/>
-      <c r="H18" s="58" t="s">
-        <v>37</v>
-      </c>
+      <c r="H18" s="58"/>
     </row>
     <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="45"/>
@@ -1934,16 +1811,14 @@
       <c r="G19" s="62">
         <v>7607.43</v>
       </c>
-      <c r="H19" s="58" t="s">
-        <v>37</v>
-      </c>
+      <c r="H19" s="58"/>
     </row>
     <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D20" s="45"/>
       <c r="E20" s="45"/>
@@ -1951,16 +1826,14 @@
         <v>32220.7</v>
       </c>
       <c r="G20" s="46"/>
-      <c r="H20" s="58" t="s">
-        <v>35</v>
-      </c>
+      <c r="H20" s="58"/>
     </row>
     <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
@@ -1968,16 +1841,14 @@
         <v>1875</v>
       </c>
       <c r="G21" s="46"/>
-      <c r="H21" s="58" t="s">
-        <v>34</v>
-      </c>
+      <c r="H21" s="58"/>
     </row>
     <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
@@ -1985,16 +1856,14 @@
       <c r="G22" s="62">
         <v>190076.05</v>
       </c>
-      <c r="H22" s="58" t="s">
-        <v>31</v>
-      </c>
+      <c r="H22" s="58"/>
     </row>
     <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
@@ -2002,16 +1871,14 @@
       <c r="G23" s="62">
         <v>78786.53</v>
       </c>
-      <c r="H23" s="58" t="s">
-        <v>31</v>
-      </c>
+      <c r="H23" s="58"/>
     </row>
     <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -2026,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -2041,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
@@ -2049,16 +1916,14 @@
       <c r="G26" s="62">
         <v>51674.06</v>
       </c>
-      <c r="H26" s="58" t="s">
-        <v>27</v>
-      </c>
+      <c r="H26" s="58"/>
     </row>
     <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
@@ -2066,16 +1931,14 @@
       <c r="G27" s="62">
         <v>2980</v>
       </c>
-      <c r="H27" s="58" t="s">
-        <v>26</v>
-      </c>
+      <c r="H27" s="58"/>
     </row>
     <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
@@ -2083,16 +1946,14 @@
       <c r="G28" s="62">
         <v>11774.1</v>
       </c>
-      <c r="H28" s="58" t="s">
-        <v>61</v>
-      </c>
+      <c r="H28" s="58"/>
     </row>
     <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="45"/>
@@ -2100,16 +1961,14 @@
       <c r="G29" s="62">
         <v>99694</v>
       </c>
-      <c r="H29" s="58" t="s">
-        <v>62</v>
-      </c>
+      <c r="H29" s="58"/>
     </row>
     <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
@@ -2117,16 +1976,14 @@
       <c r="G30" s="62">
         <v>65000</v>
       </c>
-      <c r="H30" s="58" t="s">
-        <v>23</v>
-      </c>
+      <c r="H30" s="58"/>
     </row>
     <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
@@ -2134,16 +1991,14 @@
       <c r="G31" s="62">
         <v>138411</v>
       </c>
-      <c r="H31" s="58" t="s">
-        <v>21</v>
-      </c>
+      <c r="H31" s="58"/>
     </row>
     <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="45"/>
@@ -2151,16 +2006,14 @@
       <c r="G32" s="62">
         <v>3121988.46</v>
       </c>
-      <c r="H32" s="58" t="s">
-        <v>19</v>
-      </c>
+      <c r="H32" s="58"/>
     </row>
     <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
@@ -2168,16 +2021,14 @@
         <v>1978615.9</v>
       </c>
       <c r="G33" s="46"/>
-      <c r="H33" s="58" t="s">
-        <v>17</v>
-      </c>
+      <c r="H33" s="58"/>
     </row>
     <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
@@ -2185,14 +2036,12 @@
         <v>6850</v>
       </c>
       <c r="G34" s="46"/>
-      <c r="H34" s="58" t="s">
-        <v>67</v>
-      </c>
+      <c r="H34" s="58"/>
     </row>
     <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="43"/>
       <c r="C35" s="44" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
@@ -2200,16 +2049,14 @@
         <v>200</v>
       </c>
       <c r="G35" s="46"/>
-      <c r="H35" s="58" t="s">
-        <v>3</v>
-      </c>
+      <c r="H35" s="58"/>
     </row>
     <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
@@ -2217,16 +2064,14 @@
         <v>1231.73</v>
       </c>
       <c r="G36" s="46"/>
-      <c r="H36" s="58" t="s">
-        <v>15</v>
-      </c>
+      <c r="H36" s="58"/>
     </row>
     <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
@@ -2234,16 +2079,14 @@
         <v>900</v>
       </c>
       <c r="G37" s="46"/>
-      <c r="H37" s="58" t="s">
-        <v>68</v>
-      </c>
+      <c r="H37" s="58"/>
     </row>
     <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
@@ -2251,16 +2094,14 @@
         <v>8063.43</v>
       </c>
       <c r="G38" s="46"/>
-      <c r="H38" s="58" t="s">
-        <v>13</v>
-      </c>
+      <c r="H38" s="58"/>
     </row>
     <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
@@ -2268,14 +2109,12 @@
         <v>405.65</v>
       </c>
       <c r="G39" s="46"/>
-      <c r="H39" s="58" t="s">
-        <v>56</v>
-      </c>
+      <c r="H39" s="58"/>
     </row>
     <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
       <c r="C40" s="44" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
@@ -2283,16 +2122,14 @@
         <v>573.5</v>
       </c>
       <c r="G40" s="46"/>
-      <c r="H40" s="58" t="s">
-        <v>69</v>
-      </c>
+      <c r="H40" s="58"/>
     </row>
     <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D41" s="45"/>
       <c r="E41" s="45"/>
@@ -2300,16 +2137,14 @@
         <v>382.77</v>
       </c>
       <c r="G41" s="46"/>
-      <c r="H41" s="58" t="s">
-        <v>70</v>
-      </c>
+      <c r="H41" s="58"/>
     </row>
     <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
@@ -2317,16 +2152,14 @@
         <v>267.18</v>
       </c>
       <c r="G42" s="46"/>
-      <c r="H42" s="58" t="s">
-        <v>71</v>
-      </c>
+      <c r="H42" s="58"/>
     </row>
     <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
@@ -2334,16 +2167,14 @@
         <v>2750</v>
       </c>
       <c r="G43" s="46"/>
-      <c r="H43" s="58" t="s">
-        <v>72</v>
-      </c>
+      <c r="H43" s="58"/>
     </row>
     <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -2351,16 +2182,14 @@
         <v>1022.48</v>
       </c>
       <c r="G44" s="46"/>
-      <c r="H44" s="58" t="s">
-        <v>57</v>
-      </c>
+      <c r="H44" s="58"/>
     </row>
     <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B45" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
@@ -2368,16 +2197,14 @@
         <v>2.15</v>
       </c>
       <c r="G45" s="46"/>
-      <c r="H45" s="58" t="s">
-        <v>73</v>
-      </c>
+      <c r="H45" s="58"/>
     </row>
     <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B46" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
@@ -2385,16 +2212,14 @@
         <v>1650</v>
       </c>
       <c r="G46" s="46"/>
-      <c r="H46" s="58" t="s">
-        <v>8</v>
-      </c>
+      <c r="H46" s="58"/>
     </row>
     <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B47" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
@@ -2402,16 +2227,14 @@
         <v>1475</v>
       </c>
       <c r="G47" s="46"/>
-      <c r="H47" s="58" t="s">
-        <v>75</v>
-      </c>
+      <c r="H47" s="58"/>
     </row>
     <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
@@ -2419,16 +2242,14 @@
         <v>1200</v>
       </c>
       <c r="G48" s="46"/>
-      <c r="H48" s="58" t="s">
-        <v>77</v>
-      </c>
+      <c r="H48" s="58"/>
     </row>
     <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B49" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
@@ -2436,16 +2257,14 @@
         <v>411.95</v>
       </c>
       <c r="G49" s="46"/>
-      <c r="H49" s="58" t="s">
-        <v>78</v>
-      </c>
+      <c r="H49" s="58"/>
     </row>
     <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B50" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
@@ -2453,16 +2272,14 @@
         <v>256338.33</v>
       </c>
       <c r="G50" s="46"/>
-      <c r="H50" s="58" t="s">
-        <v>74</v>
-      </c>
+      <c r="H50" s="58"/>
     </row>
     <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B51" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
@@ -2470,16 +2287,14 @@
         <v>430</v>
       </c>
       <c r="G51" s="46"/>
-      <c r="H51" s="58" t="s">
-        <v>76</v>
-      </c>
+      <c r="H51" s="58"/>
     </row>
     <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B52" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
@@ -2487,16 +2302,14 @@
       <c r="G52" s="62">
         <v>51495.22</v>
       </c>
-      <c r="H52" s="58" t="s">
-        <v>65</v>
-      </c>
+      <c r="H52" s="58"/>
     </row>
     <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B53" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
@@ -2504,14 +2317,12 @@
       <c r="G53" s="62">
         <v>54684.19</v>
       </c>
-      <c r="H53" s="58" t="s">
-        <v>66</v>
-      </c>
+      <c r="H53" s="58"/>
     </row>
     <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B54" s="43"/>
       <c r="C54" s="44" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
@@ -2519,9 +2330,7 @@
         <v>99640.62</v>
       </c>
       <c r="G54" s="65"/>
-      <c r="H54" s="64" t="s">
-        <v>2</v>
-      </c>
+      <c r="H54" s="64"/>
     </row>
     <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B55" s="43" t="s">
@@ -2552,10 +2361,7 @@
         <f>SUM(G11:G55)</f>
         <v>3874627.04</v>
       </c>
-      <c r="H56" s="63">
-        <f>G56-F56</f>
-        <v>0</v>
-      </c>
+      <c r="H56" s="63"/>
     </row>
     <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B57" s="43" t="s">

</xml_diff>

<commit_message>
Solved the linking issue from account to sub
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88314457-D07A-4C7B-8A32-27D9C1B4B58F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E952899D-5728-4708-B02F-4C910F70178A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2015" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -33,6 +33,12 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Income Tax Expense</t>
+  </si>
+  <si>
+    <t>Administrative Expenses</t>
+  </si>
+  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
@@ -72,15 +78,27 @@
     <t>Accounting fee</t>
   </si>
   <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
     <t>Purchases</t>
   </si>
   <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Retained Profits</t>
+  </si>
+  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
@@ -90,6 +108,9 @@
     <t>Accruals</t>
   </si>
   <si>
+    <t>GST Payables</t>
+  </si>
+  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -99,6 +120,9 @@
     <t>GST Collected</t>
   </si>
   <si>
+    <t>Trade Payables</t>
+  </si>
+  <si>
     <t>Trade Payables - USD Exchange</t>
   </si>
   <si>
@@ -108,9 +132,15 @@
     <t>Prepayments</t>
   </si>
   <si>
+    <t>Deposits</t>
+  </si>
+  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
+    <t>Plant and Equipment</t>
+  </si>
+  <si>
     <t>Softwares Accum Dep'n</t>
   </si>
   <si>
@@ -123,12 +153,18 @@
     <t>Office Equipment at Cost</t>
   </si>
   <si>
+    <t>Trade Receivables</t>
+  </si>
+  <si>
     <t>Trade Receivables - USD Exchan</t>
   </si>
   <si>
     <t>Trade Receivables - USD</t>
   </si>
   <si>
+    <t>Bank Balances</t>
+  </si>
+  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -147,6 +183,15 @@
     <t>Account</t>
   </si>
   <si>
+    <t>Trial Balance</t>
+  </si>
+  <si>
+    <t>VSIG Pte. Ltd.</t>
+  </si>
+  <si>
+    <t>December 2015</t>
+  </si>
+  <si>
     <t>Amount owing to directors</t>
   </si>
   <si>
@@ -165,10 +210,58 @@
     <t>Skill Development Levy</t>
   </si>
   <si>
+    <t>Amount owing to a Shareholder</t>
+  </si>
+  <si>
+    <t>Income Tax Payables</t>
+  </si>
+  <si>
     <t>Administrative expenses</t>
   </si>
   <si>
     <t>Freight paid</t>
+  </si>
+  <si>
+    <t>Exchange Gain - Trade</t>
+  </si>
+  <si>
+    <t>Exchange Gain - Non-trade</t>
+  </si>
+  <si>
+    <t>Accounting Fee</t>
+  </si>
+  <si>
+    <t>Compilation Fee</t>
+  </si>
+  <si>
+    <t>Freight Charges</t>
+  </si>
+  <si>
+    <t>Internet Expenses</t>
+  </si>
+  <si>
+    <t>Late Penalty</t>
+  </si>
+  <si>
+    <t>Nominee Director Fee</t>
+  </si>
+  <si>
+    <t>Postage and Courier</t>
+  </si>
+  <si>
+    <t>Salaries</t>
+  </si>
+  <si>
+    <t>Secretarial Fee</t>
+  </si>
+  <si>
+    <t>Skill Development Levy &amp; SINDA</t>
+  </si>
+  <si>
+    <t>Taxation Fee</t>
+  </si>
+  <si>
+    <t>Telephone Expenses</t>
   </si>
   <si>
     <t>Income tax expenses</t>
@@ -179,9 +272,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -388,84 +481,84 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -474,22 +567,22 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -498,49 +591,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -865,7 +958,7 @@
   <dimension ref="A1:AA68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1387,9 @@
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
       <c r="H2" s="60"/>
@@ -1323,7 +1418,9 @@
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
+      <c r="E3" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="23"/>
       <c r="G3" s="24"/>
       <c r="H3" s="60"/>
@@ -1352,7 +1449,9 @@
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
       <c r="H4" s="60"/>
@@ -1381,7 +1480,9 @@
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
+      <c r="E5" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
       <c r="H5" s="60"/>
@@ -1410,7 +1511,9 @@
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="E6" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
       <c r="H6" s="60"/>
@@ -1439,7 +1542,9 @@
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="26"/>
+      <c r="E7" s="26" t="s">
+        <v>52</v>
+      </c>
       <c r="F7" s="27"/>
       <c r="G7" s="28"/>
       <c r="H7" s="60"/>
@@ -1468,7 +1573,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="F8" s="27"/>
       <c r="G8" s="30"/>
       <c r="H8" s="60"/>
@@ -1527,15 +1634,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="38" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="41"/>
@@ -1564,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="45"/>
@@ -1572,7 +1679,9 @@
         <v>442930.78</v>
       </c>
       <c r="G11" s="46"/>
-      <c r="H11" s="58"/>
+      <c r="H11" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="47"/>
@@ -1599,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D12" s="45"/>
       <c r="E12" s="45"/>
@@ -1607,7 +1716,9 @@
         <v>399973.51</v>
       </c>
       <c r="G12" s="46"/>
-      <c r="H12" s="58"/>
+      <c r="H12" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -1634,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -1642,7 +1753,9 @@
         <v>165789.01999999999</v>
       </c>
       <c r="G13" s="46"/>
-      <c r="H13" s="58"/>
+      <c r="H13" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -1669,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
@@ -1677,7 +1790,9 @@
         <v>325522.73</v>
       </c>
       <c r="G14" s="46"/>
-      <c r="H14" s="58"/>
+      <c r="H14" s="58" t="s">
+        <v>42</v>
+      </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1704,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
@@ -1712,7 +1827,9 @@
         <v>134929.18</v>
       </c>
       <c r="G15" s="46"/>
-      <c r="H15" s="58"/>
+      <c r="H15" s="58" t="s">
+        <v>42</v>
+      </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -1739,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
@@ -1747,7 +1864,9 @@
         <v>1368</v>
       </c>
       <c r="G16" s="46"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="58" t="s">
+        <v>37</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -1773,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
@@ -1781,14 +1900,16 @@
       <c r="G17" s="62">
         <v>456</v>
       </c>
-      <c r="H17" s="58"/>
+      <c r="H17" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
@@ -1796,14 +1917,16 @@
         <v>7607.43</v>
       </c>
       <c r="G18" s="46"/>
-      <c r="H18" s="58"/>
+      <c r="H18" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="45"/>
@@ -1811,14 +1934,16 @@
       <c r="G19" s="62">
         <v>7607.43</v>
       </c>
-      <c r="H19" s="58"/>
+      <c r="H19" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D20" s="45"/>
       <c r="E20" s="45"/>
@@ -1826,14 +1951,16 @@
         <v>32220.7</v>
       </c>
       <c r="G20" s="46"/>
-      <c r="H20" s="58"/>
+      <c r="H20" s="58" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
@@ -1841,14 +1968,16 @@
         <v>1875</v>
       </c>
       <c r="G21" s="46"/>
-      <c r="H21" s="58"/>
+      <c r="H21" s="58" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
@@ -1856,14 +1985,16 @@
       <c r="G22" s="62">
         <v>190076.05</v>
       </c>
-      <c r="H22" s="58"/>
+      <c r="H22" s="58" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
@@ -1871,14 +2002,16 @@
       <c r="G23" s="62">
         <v>78786.53</v>
       </c>
-      <c r="H23" s="58"/>
+      <c r="H23" s="58" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -1893,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -1908,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
@@ -1916,14 +2049,16 @@
       <c r="G26" s="62">
         <v>51674.06</v>
       </c>
-      <c r="H26" s="58"/>
+      <c r="H26" s="58" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
@@ -1931,14 +2066,16 @@
       <c r="G27" s="62">
         <v>2980</v>
       </c>
-      <c r="H27" s="58"/>
+      <c r="H27" s="58" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
@@ -1946,14 +2083,16 @@
       <c r="G28" s="62">
         <v>11774.1</v>
       </c>
-      <c r="H28" s="58"/>
+      <c r="H28" s="58" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="45"/>
@@ -1961,14 +2100,16 @@
       <c r="G29" s="62">
         <v>99694</v>
       </c>
-      <c r="H29" s="58"/>
+      <c r="H29" s="58" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
@@ -1976,14 +2117,16 @@
       <c r="G30" s="62">
         <v>65000</v>
       </c>
-      <c r="H30" s="58"/>
+      <c r="H30" s="58" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
@@ -1991,14 +2134,16 @@
       <c r="G31" s="62">
         <v>138411</v>
       </c>
-      <c r="H31" s="58"/>
+      <c r="H31" s="58" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="45"/>
@@ -2006,14 +2151,16 @@
       <c r="G32" s="62">
         <v>3121988.46</v>
       </c>
-      <c r="H32" s="58"/>
+      <c r="H32" s="58" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
@@ -2021,14 +2168,16 @@
         <v>1978615.9</v>
       </c>
       <c r="G33" s="46"/>
-      <c r="H33" s="58"/>
+      <c r="H33" s="58" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
@@ -2036,12 +2185,14 @@
         <v>6850</v>
       </c>
       <c r="G34" s="46"/>
-      <c r="H34" s="58"/>
+      <c r="H34" s="58" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="43"/>
       <c r="C35" s="44" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
@@ -2049,14 +2200,16 @@
         <v>200</v>
       </c>
       <c r="G35" s="46"/>
-      <c r="H35" s="58"/>
+      <c r="H35" s="58" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
@@ -2064,14 +2217,16 @@
         <v>1231.73</v>
       </c>
       <c r="G36" s="46"/>
-      <c r="H36" s="58"/>
+      <c r="H36" s="58" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
@@ -2079,14 +2234,16 @@
         <v>900</v>
       </c>
       <c r="G37" s="46"/>
-      <c r="H37" s="58"/>
+      <c r="H37" s="58" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
@@ -2094,14 +2251,16 @@
         <v>8063.43</v>
       </c>
       <c r="G38" s="46"/>
-      <c r="H38" s="58"/>
+      <c r="H38" s="58" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
@@ -2109,12 +2268,14 @@
         <v>405.65</v>
       </c>
       <c r="G39" s="46"/>
-      <c r="H39" s="58"/>
+      <c r="H39" s="58" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
       <c r="C40" s="44" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
@@ -2122,14 +2283,16 @@
         <v>573.5</v>
       </c>
       <c r="G40" s="46"/>
-      <c r="H40" s="58"/>
+      <c r="H40" s="58" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="44" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D41" s="45"/>
       <c r="E41" s="45"/>
@@ -2137,14 +2300,16 @@
         <v>382.77</v>
       </c>
       <c r="G41" s="46"/>
-      <c r="H41" s="58"/>
+      <c r="H41" s="58" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
@@ -2152,14 +2317,16 @@
         <v>267.18</v>
       </c>
       <c r="G42" s="46"/>
-      <c r="H42" s="58"/>
+      <c r="H42" s="58" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
@@ -2167,14 +2334,16 @@
         <v>2750</v>
       </c>
       <c r="G43" s="46"/>
-      <c r="H43" s="58"/>
+      <c r="H43" s="58" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -2182,14 +2351,16 @@
         <v>1022.48</v>
       </c>
       <c r="G44" s="46"/>
-      <c r="H44" s="58"/>
+      <c r="H44" s="58" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B45" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
@@ -2197,14 +2368,16 @@
         <v>2.15</v>
       </c>
       <c r="G45" s="46"/>
-      <c r="H45" s="58"/>
+      <c r="H45" s="58" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B46" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
@@ -2212,14 +2385,16 @@
         <v>1650</v>
       </c>
       <c r="G46" s="46"/>
-      <c r="H46" s="58"/>
+      <c r="H46" s="58" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B47" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
@@ -2227,14 +2402,16 @@
         <v>1475</v>
       </c>
       <c r="G47" s="46"/>
-      <c r="H47" s="58"/>
+      <c r="H47" s="58" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
@@ -2242,14 +2419,16 @@
         <v>1200</v>
       </c>
       <c r="G48" s="46"/>
-      <c r="H48" s="58"/>
+      <c r="H48" s="58" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B49" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
@@ -2257,14 +2436,16 @@
         <v>411.95</v>
       </c>
       <c r="G49" s="46"/>
-      <c r="H49" s="58"/>
+      <c r="H49" s="58" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B50" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
@@ -2272,14 +2453,16 @@
         <v>256338.33</v>
       </c>
       <c r="G50" s="46"/>
-      <c r="H50" s="58"/>
+      <c r="H50" s="58" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B51" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
@@ -2287,14 +2470,16 @@
         <v>430</v>
       </c>
       <c r="G51" s="46"/>
-      <c r="H51" s="58"/>
+      <c r="H51" s="58" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B52" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
@@ -2302,14 +2487,16 @@
       <c r="G52" s="62">
         <v>51495.22</v>
       </c>
-      <c r="H52" s="58"/>
+      <c r="H52" s="58" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B53" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
@@ -2317,12 +2504,14 @@
       <c r="G53" s="62">
         <v>54684.19</v>
       </c>
-      <c r="H53" s="58"/>
+      <c r="H53" s="58" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B54" s="43"/>
       <c r="C54" s="44" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
@@ -2330,7 +2519,9 @@
         <v>99640.62</v>
       </c>
       <c r="G54" s="65"/>
-      <c r="H54" s="64"/>
+      <c r="H54" s="64" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B55" s="43" t="s">
@@ -2361,7 +2552,10 @@
         <f>SUM(G11:G55)</f>
         <v>3874627.04</v>
       </c>
-      <c r="H56" s="63"/>
+      <c r="H56" s="63">
+        <f>G56-F56</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B57" s="43" t="s">

</xml_diff>

<commit_message>
Fixed some categorising issue
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E952899D-5728-4708-B02F-4C910F70178A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88314457-D07A-4C7B-8A32-27D9C1B4B58F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2015" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
   <si>
     <t/>
   </si>
@@ -33,12 +33,6 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Income Tax Expense</t>
-  </si>
-  <si>
-    <t>Administrative Expenses</t>
-  </si>
-  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
@@ -78,27 +72,15 @@
     <t>Accounting fee</t>
   </si>
   <si>
-    <t>Cost of Sales</t>
-  </si>
-  <si>
     <t>Purchases</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>Retained Profits</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
-    <t>Share Capital</t>
-  </si>
-  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
@@ -108,9 +90,6 @@
     <t>Accruals</t>
   </si>
   <si>
-    <t>GST Payables</t>
-  </si>
-  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -120,9 +99,6 @@
     <t>GST Collected</t>
   </si>
   <si>
-    <t>Trade Payables</t>
-  </si>
-  <si>
     <t>Trade Payables - USD Exchange</t>
   </si>
   <si>
@@ -132,15 +108,9 @@
     <t>Prepayments</t>
   </si>
   <si>
-    <t>Deposits</t>
-  </si>
-  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
-    <t>Plant and Equipment</t>
-  </si>
-  <si>
     <t>Softwares Accum Dep'n</t>
   </si>
   <si>
@@ -153,18 +123,12 @@
     <t>Office Equipment at Cost</t>
   </si>
   <si>
-    <t>Trade Receivables</t>
-  </si>
-  <si>
     <t>Trade Receivables - USD Exchan</t>
   </si>
   <si>
     <t>Trade Receivables - USD</t>
   </si>
   <si>
-    <t>Bank Balances</t>
-  </si>
-  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -183,15 +147,6 @@
     <t>Account</t>
   </si>
   <si>
-    <t>Trial Balance</t>
-  </si>
-  <si>
-    <t>VSIG Pte. Ltd.</t>
-  </si>
-  <si>
-    <t>December 2015</t>
-  </si>
-  <si>
     <t>Amount owing to directors</t>
   </si>
   <si>
@@ -210,58 +165,10 @@
     <t>Skill Development Levy</t>
   </si>
   <si>
-    <t>Amount owing to a Shareholder</t>
-  </si>
-  <si>
-    <t>Income Tax Payables</t>
-  </si>
-  <si>
     <t>Administrative expenses</t>
   </si>
   <si>
     <t>Freight paid</t>
-  </si>
-  <si>
-    <t>Exchange Gain - Trade</t>
-  </si>
-  <si>
-    <t>Exchange Gain - Non-trade</t>
-  </si>
-  <si>
-    <t>Accounting Fee</t>
-  </si>
-  <si>
-    <t>Compilation Fee</t>
-  </si>
-  <si>
-    <t>Freight Charges</t>
-  </si>
-  <si>
-    <t>Internet Expenses</t>
-  </si>
-  <si>
-    <t>Late Penalty</t>
-  </si>
-  <si>
-    <t>Nominee Director Fee</t>
-  </si>
-  <si>
-    <t>Postage and Courier</t>
-  </si>
-  <si>
-    <t>Salaries</t>
-  </si>
-  <si>
-    <t>Secretarial Fee</t>
-  </si>
-  <si>
-    <t>Skill Development Levy &amp; SINDA</t>
-  </si>
-  <si>
-    <t>Taxation Fee</t>
-  </si>
-  <si>
-    <t>Telephone Expenses</t>
   </si>
   <si>
     <t>Income tax expenses</t>
@@ -272,9 +179,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -481,84 +388,84 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,22 +474,22 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -591,49 +498,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -958,7 +865,7 @@
   <dimension ref="A1:AA68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1387,9 +1294,7 @@
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="16" t="s">
-        <v>53</v>
-      </c>
+      <c r="E2" s="16"/>
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
       <c r="H2" s="60"/>
@@ -1418,9 +1323,7 @@
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="22"/>
       <c r="F3" s="23"/>
       <c r="G3" s="24"/>
       <c r="H3" s="60"/>
@@ -1449,9 +1352,7 @@
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="D4" s="21"/>
-      <c r="E4" s="22" t="s">
-        <v>0</v>
-      </c>
+      <c r="E4" s="22"/>
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
       <c r="H4" s="60"/>
@@ -1480,9 +1381,7 @@
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="22" t="s">
-        <v>0</v>
-      </c>
+      <c r="E5" s="22"/>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
       <c r="H5" s="60"/>
@@ -1511,9 +1410,7 @@
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="22" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="22"/>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
       <c r="H6" s="60"/>
@@ -1542,9 +1439,7 @@
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="E7" s="26"/>
       <c r="F7" s="27"/>
       <c r="G7" s="28"/>
       <c r="H7" s="60"/>
@@ -1573,9 +1468,7 @@
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="29" t="s">
-        <v>54</v>
-      </c>
+      <c r="E8" s="29"/>
       <c r="F8" s="27"/>
       <c r="G8" s="30"/>
       <c r="H8" s="60"/>
@@ -1634,15 +1527,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="38" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="41"/>
@@ -1671,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="45"/>
@@ -1679,9 +1572,7 @@
         <v>442930.78</v>
       </c>
       <c r="G11" s="46"/>
-      <c r="H11" s="58" t="s">
-        <v>45</v>
-      </c>
+      <c r="H11" s="58"/>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="47"/>
@@ -1708,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D12" s="45"/>
       <c r="E12" s="45"/>
@@ -1716,9 +1607,7 @@
         <v>399973.51</v>
       </c>
       <c r="G12" s="46"/>
-      <c r="H12" s="58" t="s">
-        <v>45</v>
-      </c>
+      <c r="H12" s="58"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -1745,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -1753,9 +1642,7 @@
         <v>165789.01999999999</v>
       </c>
       <c r="G13" s="46"/>
-      <c r="H13" s="58" t="s">
-        <v>45</v>
-      </c>
+      <c r="H13" s="58"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -1782,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
@@ -1790,9 +1677,7 @@
         <v>325522.73</v>
       </c>
       <c r="G14" s="46"/>
-      <c r="H14" s="58" t="s">
-        <v>42</v>
-      </c>
+      <c r="H14" s="58"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1819,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
@@ -1827,9 +1712,7 @@
         <v>134929.18</v>
       </c>
       <c r="G15" s="46"/>
-      <c r="H15" s="58" t="s">
-        <v>42</v>
-      </c>
+      <c r="H15" s="58"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -1856,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
@@ -1864,9 +1747,7 @@
         <v>1368</v>
       </c>
       <c r="G16" s="46"/>
-      <c r="H16" s="58" t="s">
-        <v>37</v>
-      </c>
+      <c r="H16" s="58"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -1892,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
@@ -1900,16 +1781,14 @@
       <c r="G17" s="62">
         <v>456</v>
       </c>
-      <c r="H17" s="58" t="s">
-        <v>37</v>
-      </c>
+      <c r="H17" s="58"/>
     </row>
     <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
@@ -1917,16 +1796,14 @@
         <v>7607.43</v>
       </c>
       <c r="G18" s="46"/>
-      <c r="H18" s="58" t="s">
-        <v>37</v>
-      </c>
+      <c r="H18" s="58"/>
     </row>
     <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="45"/>
@@ -1934,16 +1811,14 @@
       <c r="G19" s="62">
         <v>7607.43</v>
       </c>
-      <c r="H19" s="58" t="s">
-        <v>37</v>
-      </c>
+      <c r="H19" s="58"/>
     </row>
     <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D20" s="45"/>
       <c r="E20" s="45"/>
@@ -1951,16 +1826,14 @@
         <v>32220.7</v>
       </c>
       <c r="G20" s="46"/>
-      <c r="H20" s="58" t="s">
-        <v>35</v>
-      </c>
+      <c r="H20" s="58"/>
     </row>
     <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
@@ -1968,16 +1841,14 @@
         <v>1875</v>
       </c>
       <c r="G21" s="46"/>
-      <c r="H21" s="58" t="s">
-        <v>34</v>
-      </c>
+      <c r="H21" s="58"/>
     </row>
     <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
@@ -1985,16 +1856,14 @@
       <c r="G22" s="62">
         <v>190076.05</v>
       </c>
-      <c r="H22" s="58" t="s">
-        <v>31</v>
-      </c>
+      <c r="H22" s="58"/>
     </row>
     <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
@@ -2002,16 +1871,14 @@
       <c r="G23" s="62">
         <v>78786.53</v>
       </c>
-      <c r="H23" s="58" t="s">
-        <v>31</v>
-      </c>
+      <c r="H23" s="58"/>
     </row>
     <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -2026,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -2041,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
@@ -2049,16 +1916,14 @@
       <c r="G26" s="62">
         <v>51674.06</v>
       </c>
-      <c r="H26" s="58" t="s">
-        <v>27</v>
-      </c>
+      <c r="H26" s="58"/>
     </row>
     <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
@@ -2066,16 +1931,14 @@
       <c r="G27" s="62">
         <v>2980</v>
       </c>
-      <c r="H27" s="58" t="s">
-        <v>26</v>
-      </c>
+      <c r="H27" s="58"/>
     </row>
     <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
@@ -2083,16 +1946,14 @@
       <c r="G28" s="62">
         <v>11774.1</v>
       </c>
-      <c r="H28" s="58" t="s">
-        <v>61</v>
-      </c>
+      <c r="H28" s="58"/>
     </row>
     <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="45"/>
@@ -2100,16 +1961,14 @@
       <c r="G29" s="62">
         <v>99694</v>
       </c>
-      <c r="H29" s="58" t="s">
-        <v>62</v>
-      </c>
+      <c r="H29" s="58"/>
     </row>
     <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
@@ -2117,16 +1976,14 @@
       <c r="G30" s="62">
         <v>65000</v>
       </c>
-      <c r="H30" s="58" t="s">
-        <v>23</v>
-      </c>
+      <c r="H30" s="58"/>
     </row>
     <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
@@ -2134,16 +1991,14 @@
       <c r="G31" s="62">
         <v>138411</v>
       </c>
-      <c r="H31" s="58" t="s">
-        <v>21</v>
-      </c>
+      <c r="H31" s="58"/>
     </row>
     <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="45"/>
@@ -2151,16 +2006,14 @@
       <c r="G32" s="62">
         <v>3121988.46</v>
       </c>
-      <c r="H32" s="58" t="s">
-        <v>19</v>
-      </c>
+      <c r="H32" s="58"/>
     </row>
     <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
@@ -2168,16 +2021,14 @@
         <v>1978615.9</v>
       </c>
       <c r="G33" s="46"/>
-      <c r="H33" s="58" t="s">
-        <v>17</v>
-      </c>
+      <c r="H33" s="58"/>
     </row>
     <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
@@ -2185,14 +2036,12 @@
         <v>6850</v>
       </c>
       <c r="G34" s="46"/>
-      <c r="H34" s="58" t="s">
-        <v>67</v>
-      </c>
+      <c r="H34" s="58"/>
     </row>
     <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="43"/>
       <c r="C35" s="44" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
@@ -2200,16 +2049,14 @@
         <v>200</v>
       </c>
       <c r="G35" s="46"/>
-      <c r="H35" s="58" t="s">
-        <v>3</v>
-      </c>
+      <c r="H35" s="58"/>
     </row>
     <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
@@ -2217,16 +2064,14 @@
         <v>1231.73</v>
       </c>
       <c r="G36" s="46"/>
-      <c r="H36" s="58" t="s">
-        <v>15</v>
-      </c>
+      <c r="H36" s="58"/>
     </row>
     <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
@@ -2234,16 +2079,14 @@
         <v>900</v>
       </c>
       <c r="G37" s="46"/>
-      <c r="H37" s="58" t="s">
-        <v>68</v>
-      </c>
+      <c r="H37" s="58"/>
     </row>
     <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
@@ -2251,16 +2094,14 @@
         <v>8063.43</v>
       </c>
       <c r="G38" s="46"/>
-      <c r="H38" s="58" t="s">
-        <v>13</v>
-      </c>
+      <c r="H38" s="58"/>
     </row>
     <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
@@ -2268,14 +2109,12 @@
         <v>405.65</v>
       </c>
       <c r="G39" s="46"/>
-      <c r="H39" s="58" t="s">
-        <v>56</v>
-      </c>
+      <c r="H39" s="58"/>
     </row>
     <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
       <c r="C40" s="44" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
@@ -2283,16 +2122,14 @@
         <v>573.5</v>
       </c>
       <c r="G40" s="46"/>
-      <c r="H40" s="58" t="s">
-        <v>69</v>
-      </c>
+      <c r="H40" s="58"/>
     </row>
     <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D41" s="45"/>
       <c r="E41" s="45"/>
@@ -2300,16 +2137,14 @@
         <v>382.77</v>
       </c>
       <c r="G41" s="46"/>
-      <c r="H41" s="58" t="s">
-        <v>70</v>
-      </c>
+      <c r="H41" s="58"/>
     </row>
     <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
@@ -2317,16 +2152,14 @@
         <v>267.18</v>
       </c>
       <c r="G42" s="46"/>
-      <c r="H42" s="58" t="s">
-        <v>71</v>
-      </c>
+      <c r="H42" s="58"/>
     </row>
     <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
@@ -2334,16 +2167,14 @@
         <v>2750</v>
       </c>
       <c r="G43" s="46"/>
-      <c r="H43" s="58" t="s">
-        <v>72</v>
-      </c>
+      <c r="H43" s="58"/>
     </row>
     <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -2351,16 +2182,14 @@
         <v>1022.48</v>
       </c>
       <c r="G44" s="46"/>
-      <c r="H44" s="58" t="s">
-        <v>57</v>
-      </c>
+      <c r="H44" s="58"/>
     </row>
     <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B45" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
@@ -2368,16 +2197,14 @@
         <v>2.15</v>
       </c>
       <c r="G45" s="46"/>
-      <c r="H45" s="58" t="s">
-        <v>73</v>
-      </c>
+      <c r="H45" s="58"/>
     </row>
     <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B46" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
@@ -2385,16 +2212,14 @@
         <v>1650</v>
       </c>
       <c r="G46" s="46"/>
-      <c r="H46" s="58" t="s">
-        <v>8</v>
-      </c>
+      <c r="H46" s="58"/>
     </row>
     <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B47" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
@@ -2402,16 +2227,14 @@
         <v>1475</v>
       </c>
       <c r="G47" s="46"/>
-      <c r="H47" s="58" t="s">
-        <v>75</v>
-      </c>
+      <c r="H47" s="58"/>
     </row>
     <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
@@ -2419,16 +2242,14 @@
         <v>1200</v>
       </c>
       <c r="G48" s="46"/>
-      <c r="H48" s="58" t="s">
-        <v>77</v>
-      </c>
+      <c r="H48" s="58"/>
     </row>
     <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B49" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
@@ -2436,16 +2257,14 @@
         <v>411.95</v>
       </c>
       <c r="G49" s="46"/>
-      <c r="H49" s="58" t="s">
-        <v>78</v>
-      </c>
+      <c r="H49" s="58"/>
     </row>
     <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B50" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
@@ -2453,16 +2272,14 @@
         <v>256338.33</v>
       </c>
       <c r="G50" s="46"/>
-      <c r="H50" s="58" t="s">
-        <v>74</v>
-      </c>
+      <c r="H50" s="58"/>
     </row>
     <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B51" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
@@ -2470,16 +2287,14 @@
         <v>430</v>
       </c>
       <c r="G51" s="46"/>
-      <c r="H51" s="58" t="s">
-        <v>76</v>
-      </c>
+      <c r="H51" s="58"/>
     </row>
     <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B52" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
@@ -2487,16 +2302,14 @@
       <c r="G52" s="62">
         <v>51495.22</v>
       </c>
-      <c r="H52" s="58" t="s">
-        <v>65</v>
-      </c>
+      <c r="H52" s="58"/>
     </row>
     <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B53" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
@@ -2504,14 +2317,12 @@
       <c r="G53" s="62">
         <v>54684.19</v>
       </c>
-      <c r="H53" s="58" t="s">
-        <v>66</v>
-      </c>
+      <c r="H53" s="58"/>
     </row>
     <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B54" s="43"/>
       <c r="C54" s="44" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
@@ -2519,9 +2330,7 @@
         <v>99640.62</v>
       </c>
       <c r="G54" s="65"/>
-      <c r="H54" s="64" t="s">
-        <v>2</v>
-      </c>
+      <c r="H54" s="64"/>
     </row>
     <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B55" s="43" t="s">
@@ -2552,10 +2361,7 @@
         <f>SUM(G11:G55)</f>
         <v>3874627.04</v>
       </c>
-      <c r="H56" s="63">
-        <f>G56-F56</f>
-        <v>0</v>
-      </c>
+      <c r="H56" s="63"/>
     </row>
     <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B57" s="43" t="s">

</xml_diff>

<commit_message>
Changed category main logic part
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88314457-D07A-4C7B-8A32-27D9C1B4B58F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E952899D-5728-4708-B02F-4C910F70178A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2015" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -33,6 +33,12 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Income Tax Expense</t>
+  </si>
+  <si>
+    <t>Administrative Expenses</t>
+  </si>
+  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
@@ -72,15 +78,27 @@
     <t>Accounting fee</t>
   </si>
   <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
     <t>Purchases</t>
   </si>
   <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Retained Profits</t>
+  </si>
+  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
@@ -90,6 +108,9 @@
     <t>Accruals</t>
   </si>
   <si>
+    <t>GST Payables</t>
+  </si>
+  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -99,6 +120,9 @@
     <t>GST Collected</t>
   </si>
   <si>
+    <t>Trade Payables</t>
+  </si>
+  <si>
     <t>Trade Payables - USD Exchange</t>
   </si>
   <si>
@@ -108,9 +132,15 @@
     <t>Prepayments</t>
   </si>
   <si>
+    <t>Deposits</t>
+  </si>
+  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
+    <t>Plant and Equipment</t>
+  </si>
+  <si>
     <t>Softwares Accum Dep'n</t>
   </si>
   <si>
@@ -123,12 +153,18 @@
     <t>Office Equipment at Cost</t>
   </si>
   <si>
+    <t>Trade Receivables</t>
+  </si>
+  <si>
     <t>Trade Receivables - USD Exchan</t>
   </si>
   <si>
     <t>Trade Receivables - USD</t>
   </si>
   <si>
+    <t>Bank Balances</t>
+  </si>
+  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -147,6 +183,15 @@
     <t>Account</t>
   </si>
   <si>
+    <t>Trial Balance</t>
+  </si>
+  <si>
+    <t>VSIG Pte. Ltd.</t>
+  </si>
+  <si>
+    <t>December 2015</t>
+  </si>
+  <si>
     <t>Amount owing to directors</t>
   </si>
   <si>
@@ -165,10 +210,58 @@
     <t>Skill Development Levy</t>
   </si>
   <si>
+    <t>Amount owing to a Shareholder</t>
+  </si>
+  <si>
+    <t>Income Tax Payables</t>
+  </si>
+  <si>
     <t>Administrative expenses</t>
   </si>
   <si>
     <t>Freight paid</t>
+  </si>
+  <si>
+    <t>Exchange Gain - Trade</t>
+  </si>
+  <si>
+    <t>Exchange Gain - Non-trade</t>
+  </si>
+  <si>
+    <t>Accounting Fee</t>
+  </si>
+  <si>
+    <t>Compilation Fee</t>
+  </si>
+  <si>
+    <t>Freight Charges</t>
+  </si>
+  <si>
+    <t>Internet Expenses</t>
+  </si>
+  <si>
+    <t>Late Penalty</t>
+  </si>
+  <si>
+    <t>Nominee Director Fee</t>
+  </si>
+  <si>
+    <t>Postage and Courier</t>
+  </si>
+  <si>
+    <t>Salaries</t>
+  </si>
+  <si>
+    <t>Secretarial Fee</t>
+  </si>
+  <si>
+    <t>Skill Development Levy &amp; SINDA</t>
+  </si>
+  <si>
+    <t>Taxation Fee</t>
+  </si>
+  <si>
+    <t>Telephone Expenses</t>
   </si>
   <si>
     <t>Income tax expenses</t>
@@ -179,9 +272,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -388,84 +481,84 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -474,22 +567,22 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -498,49 +591,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -865,7 +958,7 @@
   <dimension ref="A1:AA68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1387,9 @@
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
       <c r="H2" s="60"/>
@@ -1323,7 +1418,9 @@
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
+      <c r="E3" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="23"/>
       <c r="G3" s="24"/>
       <c r="H3" s="60"/>
@@ -1352,7 +1449,9 @@
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
       <c r="H4" s="60"/>
@@ -1381,7 +1480,9 @@
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
+      <c r="E5" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
       <c r="H5" s="60"/>
@@ -1410,7 +1511,9 @@
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="E6" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
       <c r="H6" s="60"/>
@@ -1439,7 +1542,9 @@
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="26"/>
+      <c r="E7" s="26" t="s">
+        <v>52</v>
+      </c>
       <c r="F7" s="27"/>
       <c r="G7" s="28"/>
       <c r="H7" s="60"/>
@@ -1468,7 +1573,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="F8" s="27"/>
       <c r="G8" s="30"/>
       <c r="H8" s="60"/>
@@ -1527,15 +1634,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="38" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="41"/>
@@ -1564,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="45"/>
@@ -1572,7 +1679,9 @@
         <v>442930.78</v>
       </c>
       <c r="G11" s="46"/>
-      <c r="H11" s="58"/>
+      <c r="H11" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="47"/>
@@ -1599,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D12" s="45"/>
       <c r="E12" s="45"/>
@@ -1607,7 +1716,9 @@
         <v>399973.51</v>
       </c>
       <c r="G12" s="46"/>
-      <c r="H12" s="58"/>
+      <c r="H12" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -1634,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -1642,7 +1753,9 @@
         <v>165789.01999999999</v>
       </c>
       <c r="G13" s="46"/>
-      <c r="H13" s="58"/>
+      <c r="H13" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -1669,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
@@ -1677,7 +1790,9 @@
         <v>325522.73</v>
       </c>
       <c r="G14" s="46"/>
-      <c r="H14" s="58"/>
+      <c r="H14" s="58" t="s">
+        <v>42</v>
+      </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1704,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
@@ -1712,7 +1827,9 @@
         <v>134929.18</v>
       </c>
       <c r="G15" s="46"/>
-      <c r="H15" s="58"/>
+      <c r="H15" s="58" t="s">
+        <v>42</v>
+      </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -1739,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
@@ -1747,7 +1864,9 @@
         <v>1368</v>
       </c>
       <c r="G16" s="46"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="58" t="s">
+        <v>37</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -1773,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
@@ -1781,14 +1900,16 @@
       <c r="G17" s="62">
         <v>456</v>
       </c>
-      <c r="H17" s="58"/>
+      <c r="H17" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
@@ -1796,14 +1917,16 @@
         <v>7607.43</v>
       </c>
       <c r="G18" s="46"/>
-      <c r="H18" s="58"/>
+      <c r="H18" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="45"/>
@@ -1811,14 +1934,16 @@
       <c r="G19" s="62">
         <v>7607.43</v>
       </c>
-      <c r="H19" s="58"/>
+      <c r="H19" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D20" s="45"/>
       <c r="E20" s="45"/>
@@ -1826,14 +1951,16 @@
         <v>32220.7</v>
       </c>
       <c r="G20" s="46"/>
-      <c r="H20" s="58"/>
+      <c r="H20" s="58" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
@@ -1841,14 +1968,16 @@
         <v>1875</v>
       </c>
       <c r="G21" s="46"/>
-      <c r="H21" s="58"/>
+      <c r="H21" s="58" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
@@ -1856,14 +1985,16 @@
       <c r="G22" s="62">
         <v>190076.05</v>
       </c>
-      <c r="H22" s="58"/>
+      <c r="H22" s="58" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
@@ -1871,14 +2002,16 @@
       <c r="G23" s="62">
         <v>78786.53</v>
       </c>
-      <c r="H23" s="58"/>
+      <c r="H23" s="58" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -1893,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -1908,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
@@ -1916,14 +2049,16 @@
       <c r="G26" s="62">
         <v>51674.06</v>
       </c>
-      <c r="H26" s="58"/>
+      <c r="H26" s="58" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
@@ -1931,14 +2066,16 @@
       <c r="G27" s="62">
         <v>2980</v>
       </c>
-      <c r="H27" s="58"/>
+      <c r="H27" s="58" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
@@ -1946,14 +2083,16 @@
       <c r="G28" s="62">
         <v>11774.1</v>
       </c>
-      <c r="H28" s="58"/>
+      <c r="H28" s="58" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="45"/>
@@ -1961,14 +2100,16 @@
       <c r="G29" s="62">
         <v>99694</v>
       </c>
-      <c r="H29" s="58"/>
+      <c r="H29" s="58" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
@@ -1976,14 +2117,16 @@
       <c r="G30" s="62">
         <v>65000</v>
       </c>
-      <c r="H30" s="58"/>
+      <c r="H30" s="58" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
@@ -1991,14 +2134,16 @@
       <c r="G31" s="62">
         <v>138411</v>
       </c>
-      <c r="H31" s="58"/>
+      <c r="H31" s="58" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="45"/>
@@ -2006,14 +2151,16 @@
       <c r="G32" s="62">
         <v>3121988.46</v>
       </c>
-      <c r="H32" s="58"/>
+      <c r="H32" s="58" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
@@ -2021,14 +2168,16 @@
         <v>1978615.9</v>
       </c>
       <c r="G33" s="46"/>
-      <c r="H33" s="58"/>
+      <c r="H33" s="58" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
@@ -2036,12 +2185,14 @@
         <v>6850</v>
       </c>
       <c r="G34" s="46"/>
-      <c r="H34" s="58"/>
+      <c r="H34" s="58" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="43"/>
       <c r="C35" s="44" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
@@ -2049,14 +2200,16 @@
         <v>200</v>
       </c>
       <c r="G35" s="46"/>
-      <c r="H35" s="58"/>
+      <c r="H35" s="58" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
@@ -2064,14 +2217,16 @@
         <v>1231.73</v>
       </c>
       <c r="G36" s="46"/>
-      <c r="H36" s="58"/>
+      <c r="H36" s="58" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
@@ -2079,14 +2234,16 @@
         <v>900</v>
       </c>
       <c r="G37" s="46"/>
-      <c r="H37" s="58"/>
+      <c r="H37" s="58" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
@@ -2094,14 +2251,16 @@
         <v>8063.43</v>
       </c>
       <c r="G38" s="46"/>
-      <c r="H38" s="58"/>
+      <c r="H38" s="58" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
@@ -2109,12 +2268,14 @@
         <v>405.65</v>
       </c>
       <c r="G39" s="46"/>
-      <c r="H39" s="58"/>
+      <c r="H39" s="58" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
       <c r="C40" s="44" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
@@ -2122,14 +2283,16 @@
         <v>573.5</v>
       </c>
       <c r="G40" s="46"/>
-      <c r="H40" s="58"/>
+      <c r="H40" s="58" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="44" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D41" s="45"/>
       <c r="E41" s="45"/>
@@ -2137,14 +2300,16 @@
         <v>382.77</v>
       </c>
       <c r="G41" s="46"/>
-      <c r="H41" s="58"/>
+      <c r="H41" s="58" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
@@ -2152,14 +2317,16 @@
         <v>267.18</v>
       </c>
       <c r="G42" s="46"/>
-      <c r="H42" s="58"/>
+      <c r="H42" s="58" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
@@ -2167,14 +2334,16 @@
         <v>2750</v>
       </c>
       <c r="G43" s="46"/>
-      <c r="H43" s="58"/>
+      <c r="H43" s="58" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -2182,14 +2351,16 @@
         <v>1022.48</v>
       </c>
       <c r="G44" s="46"/>
-      <c r="H44" s="58"/>
+      <c r="H44" s="58" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B45" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
@@ -2197,14 +2368,16 @@
         <v>2.15</v>
       </c>
       <c r="G45" s="46"/>
-      <c r="H45" s="58"/>
+      <c r="H45" s="58" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B46" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
@@ -2212,14 +2385,16 @@
         <v>1650</v>
       </c>
       <c r="G46" s="46"/>
-      <c r="H46" s="58"/>
+      <c r="H46" s="58" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B47" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
@@ -2227,14 +2402,16 @@
         <v>1475</v>
       </c>
       <c r="G47" s="46"/>
-      <c r="H47" s="58"/>
+      <c r="H47" s="58" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
@@ -2242,14 +2419,16 @@
         <v>1200</v>
       </c>
       <c r="G48" s="46"/>
-      <c r="H48" s="58"/>
+      <c r="H48" s="58" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B49" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
@@ -2257,14 +2436,16 @@
         <v>411.95</v>
       </c>
       <c r="G49" s="46"/>
-      <c r="H49" s="58"/>
+      <c r="H49" s="58" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B50" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
@@ -2272,14 +2453,16 @@
         <v>256338.33</v>
       </c>
       <c r="G50" s="46"/>
-      <c r="H50" s="58"/>
+      <c r="H50" s="58" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B51" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
@@ -2287,14 +2470,16 @@
         <v>430</v>
       </c>
       <c r="G51" s="46"/>
-      <c r="H51" s="58"/>
+      <c r="H51" s="58" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B52" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
@@ -2302,14 +2487,16 @@
       <c r="G52" s="62">
         <v>51495.22</v>
       </c>
-      <c r="H52" s="58"/>
+      <c r="H52" s="58" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B53" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
@@ -2317,12 +2504,14 @@
       <c r="G53" s="62">
         <v>54684.19</v>
       </c>
-      <c r="H53" s="58"/>
+      <c r="H53" s="58" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B54" s="43"/>
       <c r="C54" s="44" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
@@ -2330,7 +2519,9 @@
         <v>99640.62</v>
       </c>
       <c r="G54" s="65"/>
-      <c r="H54" s="64"/>
+      <c r="H54" s="64" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B55" s="43" t="s">
@@ -2361,7 +2552,10 @@
         <f>SUM(G11:G55)</f>
         <v>3874627.04</v>
       </c>
-      <c r="H56" s="63"/>
+      <c r="H56" s="63">
+        <f>G56-F56</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B57" s="43" t="s">

</xml_diff>

<commit_message>
Appendix now working with database
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) second page.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88314457-D07A-4C7B-8A32-27D9C1B4B58F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E952899D-5728-4708-B02F-4C910F70178A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2015" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -33,6 +33,12 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Income Tax Expense</t>
+  </si>
+  <si>
+    <t>Administrative Expenses</t>
+  </si>
+  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
@@ -72,15 +78,27 @@
     <t>Accounting fee</t>
   </si>
   <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
     <t>Purchases</t>
   </si>
   <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Retained Profits</t>
+  </si>
+  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
@@ -90,6 +108,9 @@
     <t>Accruals</t>
   </si>
   <si>
+    <t>GST Payables</t>
+  </si>
+  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -99,6 +120,9 @@
     <t>GST Collected</t>
   </si>
   <si>
+    <t>Trade Payables</t>
+  </si>
+  <si>
     <t>Trade Payables - USD Exchange</t>
   </si>
   <si>
@@ -108,9 +132,15 @@
     <t>Prepayments</t>
   </si>
   <si>
+    <t>Deposits</t>
+  </si>
+  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
+    <t>Plant and Equipment</t>
+  </si>
+  <si>
     <t>Softwares Accum Dep'n</t>
   </si>
   <si>
@@ -123,12 +153,18 @@
     <t>Office Equipment at Cost</t>
   </si>
   <si>
+    <t>Trade Receivables</t>
+  </si>
+  <si>
     <t>Trade Receivables - USD Exchan</t>
   </si>
   <si>
     <t>Trade Receivables - USD</t>
   </si>
   <si>
+    <t>Bank Balances</t>
+  </si>
+  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -147,6 +183,15 @@
     <t>Account</t>
   </si>
   <si>
+    <t>Trial Balance</t>
+  </si>
+  <si>
+    <t>VSIG Pte. Ltd.</t>
+  </si>
+  <si>
+    <t>December 2015</t>
+  </si>
+  <si>
     <t>Amount owing to directors</t>
   </si>
   <si>
@@ -165,10 +210,58 @@
     <t>Skill Development Levy</t>
   </si>
   <si>
+    <t>Amount owing to a Shareholder</t>
+  </si>
+  <si>
+    <t>Income Tax Payables</t>
+  </si>
+  <si>
     <t>Administrative expenses</t>
   </si>
   <si>
     <t>Freight paid</t>
+  </si>
+  <si>
+    <t>Exchange Gain - Trade</t>
+  </si>
+  <si>
+    <t>Exchange Gain - Non-trade</t>
+  </si>
+  <si>
+    <t>Accounting Fee</t>
+  </si>
+  <si>
+    <t>Compilation Fee</t>
+  </si>
+  <si>
+    <t>Freight Charges</t>
+  </si>
+  <si>
+    <t>Internet Expenses</t>
+  </si>
+  <si>
+    <t>Late Penalty</t>
+  </si>
+  <si>
+    <t>Nominee Director Fee</t>
+  </si>
+  <si>
+    <t>Postage and Courier</t>
+  </si>
+  <si>
+    <t>Salaries</t>
+  </si>
+  <si>
+    <t>Secretarial Fee</t>
+  </si>
+  <si>
+    <t>Skill Development Levy &amp; SINDA</t>
+  </si>
+  <si>
+    <t>Taxation Fee</t>
+  </si>
+  <si>
+    <t>Telephone Expenses</t>
   </si>
   <si>
     <t>Income tax expenses</t>
@@ -179,9 +272,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -388,84 +481,84 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -474,22 +567,22 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -498,49 +591,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -865,7 +958,7 @@
   <dimension ref="A1:AA68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1387,9 @@
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
       <c r="H2" s="60"/>
@@ -1323,7 +1418,9 @@
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
+      <c r="E3" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="23"/>
       <c r="G3" s="24"/>
       <c r="H3" s="60"/>
@@ -1352,7 +1449,9 @@
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
       <c r="H4" s="60"/>
@@ -1381,7 +1480,9 @@
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
+      <c r="E5" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
       <c r="H5" s="60"/>
@@ -1410,7 +1511,9 @@
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="E6" s="22" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
       <c r="H6" s="60"/>
@@ -1439,7 +1542,9 @@
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="26"/>
+      <c r="E7" s="26" t="s">
+        <v>52</v>
+      </c>
       <c r="F7" s="27"/>
       <c r="G7" s="28"/>
       <c r="H7" s="60"/>
@@ -1468,7 +1573,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="F8" s="27"/>
       <c r="G8" s="30"/>
       <c r="H8" s="60"/>
@@ -1527,15 +1634,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="38" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="41"/>
@@ -1564,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="45"/>
@@ -1572,7 +1679,9 @@
         <v>442930.78</v>
       </c>
       <c r="G11" s="46"/>
-      <c r="H11" s="58"/>
+      <c r="H11" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="47"/>
@@ -1599,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D12" s="45"/>
       <c r="E12" s="45"/>
@@ -1607,7 +1716,9 @@
         <v>399973.51</v>
       </c>
       <c r="G12" s="46"/>
-      <c r="H12" s="58"/>
+      <c r="H12" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -1634,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -1642,7 +1753,9 @@
         <v>165789.01999999999</v>
       </c>
       <c r="G13" s="46"/>
-      <c r="H13" s="58"/>
+      <c r="H13" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -1669,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
@@ -1677,7 +1790,9 @@
         <v>325522.73</v>
       </c>
       <c r="G14" s="46"/>
-      <c r="H14" s="58"/>
+      <c r="H14" s="58" t="s">
+        <v>42</v>
+      </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1704,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
@@ -1712,7 +1827,9 @@
         <v>134929.18</v>
       </c>
       <c r="G15" s="46"/>
-      <c r="H15" s="58"/>
+      <c r="H15" s="58" t="s">
+        <v>42</v>
+      </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -1739,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
@@ -1747,7 +1864,9 @@
         <v>1368</v>
       </c>
       <c r="G16" s="46"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="58" t="s">
+        <v>37</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -1773,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
@@ -1781,14 +1900,16 @@
       <c r="G17" s="62">
         <v>456</v>
       </c>
-      <c r="H17" s="58"/>
+      <c r="H17" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
@@ -1796,14 +1917,16 @@
         <v>7607.43</v>
       </c>
       <c r="G18" s="46"/>
-      <c r="H18" s="58"/>
+      <c r="H18" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="45"/>
@@ -1811,14 +1934,16 @@
       <c r="G19" s="62">
         <v>7607.43</v>
       </c>
-      <c r="H19" s="58"/>
+      <c r="H19" s="58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D20" s="45"/>
       <c r="E20" s="45"/>
@@ -1826,14 +1951,16 @@
         <v>32220.7</v>
       </c>
       <c r="G20" s="46"/>
-      <c r="H20" s="58"/>
+      <c r="H20" s="58" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
@@ -1841,14 +1968,16 @@
         <v>1875</v>
       </c>
       <c r="G21" s="46"/>
-      <c r="H21" s="58"/>
+      <c r="H21" s="58" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
@@ -1856,14 +1985,16 @@
       <c r="G22" s="62">
         <v>190076.05</v>
       </c>
-      <c r="H22" s="58"/>
+      <c r="H22" s="58" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
@@ -1871,14 +2002,16 @@
       <c r="G23" s="62">
         <v>78786.53</v>
       </c>
-      <c r="H23" s="58"/>
+      <c r="H23" s="58" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -1893,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -1908,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
@@ -1916,14 +2049,16 @@
       <c r="G26" s="62">
         <v>51674.06</v>
       </c>
-      <c r="H26" s="58"/>
+      <c r="H26" s="58" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
@@ -1931,14 +2066,16 @@
       <c r="G27" s="62">
         <v>2980</v>
       </c>
-      <c r="H27" s="58"/>
+      <c r="H27" s="58" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
@@ -1946,14 +2083,16 @@
       <c r="G28" s="62">
         <v>11774.1</v>
       </c>
-      <c r="H28" s="58"/>
+      <c r="H28" s="58" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="45"/>
@@ -1961,14 +2100,16 @@
       <c r="G29" s="62">
         <v>99694</v>
       </c>
-      <c r="H29" s="58"/>
+      <c r="H29" s="58" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
@@ -1976,14 +2117,16 @@
       <c r="G30" s="62">
         <v>65000</v>
       </c>
-      <c r="H30" s="58"/>
+      <c r="H30" s="58" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
@@ -1991,14 +2134,16 @@
       <c r="G31" s="62">
         <v>138411</v>
       </c>
-      <c r="H31" s="58"/>
+      <c r="H31" s="58" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="45"/>
@@ -2006,14 +2151,16 @@
       <c r="G32" s="62">
         <v>3121988.46</v>
       </c>
-      <c r="H32" s="58"/>
+      <c r="H32" s="58" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
@@ -2021,14 +2168,16 @@
         <v>1978615.9</v>
       </c>
       <c r="G33" s="46"/>
-      <c r="H33" s="58"/>
+      <c r="H33" s="58" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
@@ -2036,12 +2185,14 @@
         <v>6850</v>
       </c>
       <c r="G34" s="46"/>
-      <c r="H34" s="58"/>
+      <c r="H34" s="58" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="43"/>
       <c r="C35" s="44" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
@@ -2049,14 +2200,16 @@
         <v>200</v>
       </c>
       <c r="G35" s="46"/>
-      <c r="H35" s="58"/>
+      <c r="H35" s="58" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
@@ -2064,14 +2217,16 @@
         <v>1231.73</v>
       </c>
       <c r="G36" s="46"/>
-      <c r="H36" s="58"/>
+      <c r="H36" s="58" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
@@ -2079,14 +2234,16 @@
         <v>900</v>
       </c>
       <c r="G37" s="46"/>
-      <c r="H37" s="58"/>
+      <c r="H37" s="58" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
@@ -2094,14 +2251,16 @@
         <v>8063.43</v>
       </c>
       <c r="G38" s="46"/>
-      <c r="H38" s="58"/>
+      <c r="H38" s="58" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
@@ -2109,12 +2268,14 @@
         <v>405.65</v>
       </c>
       <c r="G39" s="46"/>
-      <c r="H39" s="58"/>
+      <c r="H39" s="58" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
       <c r="C40" s="44" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
@@ -2122,14 +2283,16 @@
         <v>573.5</v>
       </c>
       <c r="G40" s="46"/>
-      <c r="H40" s="58"/>
+      <c r="H40" s="58" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="44" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D41" s="45"/>
       <c r="E41" s="45"/>
@@ -2137,14 +2300,16 @@
         <v>382.77</v>
       </c>
       <c r="G41" s="46"/>
-      <c r="H41" s="58"/>
+      <c r="H41" s="58" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
@@ -2152,14 +2317,16 @@
         <v>267.18</v>
       </c>
       <c r="G42" s="46"/>
-      <c r="H42" s="58"/>
+      <c r="H42" s="58" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
@@ -2167,14 +2334,16 @@
         <v>2750</v>
       </c>
       <c r="G43" s="46"/>
-      <c r="H43" s="58"/>
+      <c r="H43" s="58" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -2182,14 +2351,16 @@
         <v>1022.48</v>
       </c>
       <c r="G44" s="46"/>
-      <c r="H44" s="58"/>
+      <c r="H44" s="58" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B45" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
@@ -2197,14 +2368,16 @@
         <v>2.15</v>
       </c>
       <c r="G45" s="46"/>
-      <c r="H45" s="58"/>
+      <c r="H45" s="58" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B46" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
@@ -2212,14 +2385,16 @@
         <v>1650</v>
       </c>
       <c r="G46" s="46"/>
-      <c r="H46" s="58"/>
+      <c r="H46" s="58" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B47" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
@@ -2227,14 +2402,16 @@
         <v>1475</v>
       </c>
       <c r="G47" s="46"/>
-      <c r="H47" s="58"/>
+      <c r="H47" s="58" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
@@ -2242,14 +2419,16 @@
         <v>1200</v>
       </c>
       <c r="G48" s="46"/>
-      <c r="H48" s="58"/>
+      <c r="H48" s="58" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B49" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
@@ -2257,14 +2436,16 @@
         <v>411.95</v>
       </c>
       <c r="G49" s="46"/>
-      <c r="H49" s="58"/>
+      <c r="H49" s="58" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B50" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
@@ -2272,14 +2453,16 @@
         <v>256338.33</v>
       </c>
       <c r="G50" s="46"/>
-      <c r="H50" s="58"/>
+      <c r="H50" s="58" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B51" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
@@ -2287,14 +2470,16 @@
         <v>430</v>
       </c>
       <c r="G51" s="46"/>
-      <c r="H51" s="58"/>
+      <c r="H51" s="58" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B52" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
@@ -2302,14 +2487,16 @@
       <c r="G52" s="62">
         <v>51495.22</v>
       </c>
-      <c r="H52" s="58"/>
+      <c r="H52" s="58" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B53" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
@@ -2317,12 +2504,14 @@
       <c r="G53" s="62">
         <v>54684.19</v>
       </c>
-      <c r="H53" s="58"/>
+      <c r="H53" s="58" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B54" s="43"/>
       <c r="C54" s="44" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
@@ -2330,7 +2519,9 @@
         <v>99640.62</v>
       </c>
       <c r="G54" s="65"/>
-      <c r="H54" s="64"/>
+      <c r="H54" s="64" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B55" s="43" t="s">
@@ -2361,7 +2552,10 @@
         <f>SUM(G11:G55)</f>
         <v>3874627.04</v>
       </c>
-      <c r="H56" s="63"/>
+      <c r="H56" s="63">
+        <f>G56-F56</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B57" s="43" t="s">

</xml_diff>